<commit_message>
Added keyword planner details for quilling
</commit_message>
<xml_diff>
--- a/Research/2018/March 2018/Products/RawData/1.Quilling Tools/PR_QuillingTools.xlsx
+++ b/Research/2018/March 2018/Products/RawData/1.Quilling Tools/PR_QuillingTools.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>S.No</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>Udhayam</t>
+  </si>
+  <si>
+    <t>Keyword planner results</t>
+  </si>
+  <si>
+    <t>Searches</t>
+  </si>
+  <si>
+    <t>Competition</t>
+  </si>
+  <si>
+    <t>Quilling tools</t>
+  </si>
+  <si>
+    <t>1K-10K</t>
+  </si>
+  <si>
+    <t>Quilling Set</t>
+  </si>
+  <si>
+    <t>Paper Quilling Tools</t>
+  </si>
+  <si>
+    <t>100-1K</t>
+  </si>
+  <si>
+    <t>Quilling Kit</t>
+  </si>
+  <si>
+    <t>There appears to sufficient demand for this based on keyword planner stats analysis</t>
   </si>
 </sst>
 </file>
@@ -214,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -538,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <v>0.5</v>
@@ -955,21 +988,24 @@
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="19">
         <f>SUM(F2:F19)</f>
-        <v>78.5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -977,11 +1013,81 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>2</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>3</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>4</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -998,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated 999 for quilling tools
</commit_message>
<xml_diff>
--- a/Research/2018/March 2018/Products/RawData/1.Quilling Tools/PR_QuillingTools.xlsx
+++ b/Research/2018/March 2018/Products/RawData/1.Quilling Tools/PR_QuillingTools.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>S.No</t>
   </si>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1102,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L4"/>
+  <dimension ref="A2:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,18 +1153,7 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="16">
-        <v>43173</v>
-      </c>
-      <c r="L3">
-        <v>13</v>
-      </c>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1190,6 +1179,32 @@
       </c>
       <c r="L4">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="16">
+        <v>43175</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="16">
+        <v>43175</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>